<commit_message>
Modificando lista de itens a desenvolver
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>Itens de desenvolvimento do MP</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Melhorar a apresentação da imagem no cadastro de marcas e patentes</t>
+  </si>
+  <si>
+    <t>Problema ao cadastrar um radical para uma patente</t>
   </si>
 </sst>
 </file>
@@ -275,10 +278,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B18" activeCellId="0" pane="topLeft" sqref="B18"/>
+      <selection activeCell="A13" activeCellId="0" pane="topLeft" sqref="A13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -440,6 +443,18 @@
         <v>8</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="13">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
Melhoria na geração do boleto.
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Itens de desenvolvimento do MP</t>
   </si>
@@ -75,15 +75,28 @@
   </si>
   <si>
     <t>Problema ao cadastrar um radical para uma patente</t>
+  </si>
+  <si>
+    <t>Problema ao selecionar um procurador no cadastro de patentes</t>
+  </si>
+  <si>
+    <t>Relatórios de patente</t>
+  </si>
+  <si>
+    <t>Novo item</t>
+  </si>
+  <si>
+    <t>Em desenvolvimento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
+    <numFmt formatCode="DD/MM/YY" numFmtId="166"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -122,7 +135,7 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,14 +144,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <fgColor rgb="FFFF6633"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF23FF23"/>
         <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -176,7 +195,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -199,6 +218,14 @@
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="166" xfId="0">
+      <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
@@ -257,7 +284,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF6633"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -278,17 +305,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A13" activeCellId="0" pane="topLeft" sqref="A13:D13"/>
+      <selection activeCell="A16" activeCellId="0" pane="topLeft" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="83.2193877551021"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.015306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.0969387755102"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
@@ -411,49 +438,79 @@
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="4" t="n">
-        <v>41671</v>
+      <c r="D10" s="6" t="n">
+        <v>41615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>41615</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="12">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>41615</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="13">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6" t="n">
+        <v>41615</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="14">
+      <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <v>41615</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="15">
+      <c r="A15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="12">
-      <c r="A12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="13">
-      <c r="A13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Alteração na planilha de itens de desenvolvimento.
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Itens de desenvolvimento do MP</t>
   </si>
@@ -308,7 +308,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A16" activeCellId="0" pane="topLeft" sqref="A16"/>
+      <selection activeCell="G16" activeCellId="0" pane="topLeft" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -415,17 +415,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>41315</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="10">
@@ -439,7 +439,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>41615</v>
+        <v>41315</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="11">
@@ -453,7 +453,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>41615</v>
+        <v>41315</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="12">
@@ -467,7 +467,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>41615</v>
+        <v>41315</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="13">
@@ -481,7 +481,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="6" t="n">
-        <v>41615</v>
+        <v>41315</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="14">
@@ -495,7 +495,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="6" t="n">
-        <v>41615</v>
+        <v>41315</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="15">

</xml_diff>

<commit_message>
Atualização da planilha com novos itens
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hermes\SimpleDev\doc\Projetos\Alternativa Marcas e Patentes LTDA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="188" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="188"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="37">
   <si>
     <t>Itens de desenvolvimento do MP</t>
   </si>
@@ -86,56 +90,78 @@
     <t>Novo item</t>
   </si>
   <si>
-    <t>Em desenvolvimento</t>
+    <t>Criar nova aba do cadastro de pessoa para manter o histórico de contatos</t>
+  </si>
+  <si>
+    <t>Facilitar a visualização dos dados do cliente (atualmente ele tem q buscar uma marca ou patente para descobrir o cliente para ver os dados do mesmo</t>
+  </si>
+  <si>
+    <t>Não está carrregando o valor do SM automaticamente</t>
+  </si>
+  <si>
+    <t>Fixar filtro por marca</t>
+  </si>
+  <si>
+    <t>Problemas no cadastro do valor da manutenção (marca e patente)</t>
+  </si>
+  <si>
+    <t>Problema na visualização do relatório analítico e sintético de patente</t>
+  </si>
+  <si>
+    <t>Melhoria para enviar e-mail de patentes e marcas</t>
+  </si>
+  <si>
+    <t>Indicar no cadastro de cedente se ele é o padrão</t>
+  </si>
+  <si>
+    <t>Pré-cadastro das informações do boleto (agente financeiro etc)</t>
+  </si>
+  <si>
+    <t>Tela de quitação de boleto</t>
+  </si>
+  <si>
+    <t>Não está carregando a data de vencimento da manutenção</t>
+  </si>
+  <si>
+    <t>Erro no processamento de radicais da ultima revista</t>
+  </si>
+  <si>
+    <t>Filtro por descrição no histórico de boletos</t>
+  </si>
+  <si>
+    <t>Retirar o campo observação da grid de historico de boletos e colocar botão para quitar o boleto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
-    <numFmt formatCode="DD/MM/YY" numFmtId="166"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="15"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="12"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,15 +180,9 @@
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -170,73 +190,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-  </cellStyleXfs>
-  <cellXfs count="8">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -295,32 +275,306 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Escritório">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Escritório">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Escritório">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G16" activeCellId="0" pane="topLeft" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="83.2193877551021"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.0969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="83.28515625"/>
+    <col min="2" max="2" width="11.5703125"/>
+    <col min="3" max="3" width="25.140625"/>
+    <col min="4" max="4" width="23"/>
+    <col min="5" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.85" outlineLevel="0" r="1">
+    <row r="1" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -329,7 +583,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.25" outlineLevel="0" r="3">
+    <row r="3" spans="1:5" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -344,7 +598,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="4">
+    <row r="4" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -358,7 +612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.35" outlineLevel="0" r="5">
+    <row r="5" spans="1:5" ht="25.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -368,11 +622,11 @@
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="5">
         <v>41671</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.25" outlineLevel="0" r="6">
+    <row r="6" spans="1:5" ht="49.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -382,11 +636,11 @@
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="5">
         <v>41671</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="37.3" outlineLevel="0" r="7">
+    <row r="7" spans="1:5" ht="37.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -396,11 +650,11 @@
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="5">
         <v>41671</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.35" outlineLevel="0" r="8">
+    <row r="8" spans="1:5" ht="25.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -410,11 +664,11 @@
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="5">
         <v>41671</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="9">
+    <row r="9" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -424,11 +678,11 @@
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="6">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="10">
+    <row r="10" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -438,11 +692,11 @@
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="6">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="11">
+    <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -452,11 +706,11 @@
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="6">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="12">
+    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -466,11 +720,11 @@
       <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="6">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="13">
+    <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -480,11 +734,11 @@
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="6">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="14">
+    <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -494,21 +748,217 @@
       <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="4">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="15">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -516,10 +966,9 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Correção da letiura dos radicais da ultima revista publicada
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
@@ -195,9 +195,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify"/>
@@ -210,6 +207,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -575,348 +575,348 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="25.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4">
         <v>41671</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="49.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4">
         <v>41671</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="37.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4">
         <v>41671</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4">
         <v>41671</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6">
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5">
         <v>41315</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5">
         <v>41315</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5">
         <v>41315</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5">
         <v>41315</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5">
         <v>41315</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
         <v>41315</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="B19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="B22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="C26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -928,37 +928,37 @@
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="B28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correção de problemas diversos.
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="39">
   <si>
     <t>Itens de desenvolvimento do MP</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Retirar o campo observação da grid de historico de boletos e colocar botão para quitar o boleto</t>
+  </si>
+  <si>
+    <t>Não procede</t>
+  </si>
+  <si>
+    <t>Analisado</t>
   </si>
 </sst>
 </file>
@@ -561,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -780,35 +786,38 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -822,7 +831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -836,7 +845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -850,7 +859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
@@ -864,7 +873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -878,7 +887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
@@ -892,7 +901,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -906,21 +915,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>34</v>
       </c>
@@ -934,7 +946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
@@ -948,7 +960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Implementação do novo conceito de eventos no cadadstro de pessoa.
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -773,16 +773,16 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* Correção da paginação das grids na tela de leitura da revista de patente * Correção da formtaçãoo do número do processo da patente
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MarcasEPatentes\Projetos\Desenvolvimento\doc\Projetos\Alternativa Marcas e Patentes LTDA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="188" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="188"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
   <si>
     <t>Itens de desenvolvimento do MP</t>
   </si>
@@ -135,51 +139,46 @@
   </si>
   <si>
     <t>Não procede o botão para quitar o boleto</t>
+  </si>
+  <si>
+    <t>Cadastro das instruções do Boleto</t>
+  </si>
+  <si>
+    <t>Formatação do número do processo na tela de processos de patente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
-      <b val="true"/>
-      <sz val="15"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="4">
@@ -203,7 +202,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -211,69 +210,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -332,33 +298,307 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D32" activeCellId="0" pane="topLeft" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="83.2908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0051020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5714285714286"/>
+    <col min="1" max="1" width="83.28515625"/>
+    <col min="2" max="2" width="11.5703125"/>
+    <col min="3" max="3" width="25.140625"/>
+    <col min="4" max="4" width="23"/>
+    <col min="5" max="5" width="15.85546875"/>
+    <col min="6" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.95" outlineLevel="0" r="1">
+    <row r="1" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -367,7 +607,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.2" outlineLevel="0" r="3">
+    <row r="3" spans="1:5" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -382,7 +622,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.35" outlineLevel="0" r="4">
+    <row r="4" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -396,7 +636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.35" outlineLevel="0" r="5">
+    <row r="5" spans="1:5" ht="25.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -406,11 +646,11 @@
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="5">
         <v>41671</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.35" outlineLevel="0" r="6">
+    <row r="6" spans="1:5" ht="49.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -420,11 +660,11 @@
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="5">
         <v>41671</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="37.35" outlineLevel="0" r="7">
+    <row r="7" spans="1:5" ht="37.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -434,11 +674,11 @@
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="5">
         <v>41671</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.35" outlineLevel="0" r="8">
+    <row r="8" spans="1:5" ht="25.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -448,11 +688,11 @@
       <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="5">
         <v>41671</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.35" outlineLevel="0" r="9">
+    <row r="9" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -462,11 +702,11 @@
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="6">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.35" outlineLevel="0" r="10">
+    <row r="10" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -476,11 +716,11 @@
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="6">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="11">
+    <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -490,11 +730,11 @@
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="6">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="12">
+    <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -504,11 +744,11 @@
       <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="6">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="13">
+    <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -518,11 +758,11 @@
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D13" s="6">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="14">
+    <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -532,11 +772,11 @@
       <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="4" t="n">
+      <c r="D14" s="4">
         <v>41315</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="15">
+    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
@@ -550,7 +790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="16">
+    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>23</v>
       </c>
@@ -564,7 +804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.5" outlineLevel="0" r="17">
+    <row r="17" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
@@ -578,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="18">
+    <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
@@ -595,7 +835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="19">
+    <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>28</v>
       </c>
@@ -609,7 +849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="20">
+    <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>29</v>
       </c>
@@ -623,7 +863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="21">
+    <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
@@ -637,7 +877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="22">
+    <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>31</v>
       </c>
@@ -651,7 +891,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="23">
+    <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>32</v>
       </c>
@@ -665,7 +905,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="24">
+    <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>33</v>
       </c>
@@ -679,7 +919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="25">
+    <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
@@ -693,7 +933,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="26">
+    <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>35</v>
       </c>
@@ -710,7 +950,7 @@
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="27">
+    <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>36</v>
       </c>
@@ -724,7 +964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="28">
+    <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
@@ -738,7 +978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="29">
+    <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -753,16 +993,43 @@
       </c>
       <c r="E29" s="4" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Feito o relacionamento entre o boleto gerado e contas a receber, retirado campo observação do historico de boletos gerados, corrigido carregamento da data de vencimento ao gerar boleto pela contas a receber, atualizações no código em geral.
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MarcasEPatentes\Projetos\Desenvolvimento\doc\Projetos\Alternativa Marcas e Patentes LTDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desenvolvimento\trunk\doc\Projetos\Alternativa Marcas e Patentes LTDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="43">
   <si>
     <t>Itens de desenvolvimento do MP</t>
   </si>
@@ -138,13 +138,16 @@
     <t>Retirar o campo observação da grid de historico de boletos e colocar botão para quitar o boleto</t>
   </si>
   <si>
-    <t>Não procede o botão para quitar o boleto</t>
-  </si>
-  <si>
     <t>Cadastro das instruções do Boleto</t>
   </si>
   <si>
     <t>Formatação do número do processo na tela de processos de patente</t>
+  </si>
+  <si>
+    <t>Retirado campo Observação, porém Não procede o botão para quitar o boleto</t>
+  </si>
+  <si>
+    <t>não entendi qual seria esta descrição</t>
   </si>
 </sst>
 </file>
@@ -181,7 +184,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +203,24 @@
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -213,11 +234,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify"/>
@@ -232,6 +250,18 @@
       <alignment horizontal="justify"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
   </cellXfs>
@@ -320,9 +350,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -360,7 +390,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -432,7 +462,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -584,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -599,427 +629,430 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="3" spans="1:5" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="25.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4">
         <v>41671</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="49.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4">
         <v>41671</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="37.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4">
         <v>41671</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4">
         <v>41671</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6">
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5">
         <v>41315</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5">
         <v>41315</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5">
         <v>41315</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5">
         <v>41315</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5">
         <v>41315</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
         <v>41315</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="D18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="B19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="B23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="B24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="D26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="C27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>8</v>
+      <c r="D28" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="4" t="s">
+      <c r="B29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="B30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="7" t="s">
+      <c r="C31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementação da edição de endereço Implementação do parametros para identificação do relatório no gerador de relatório de contas a receber
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desenvolvimento\trunk\doc\Projetos\Alternativa Marcas e Patentes LTDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MarcasEPatentes\Projetos\Desenvolvimento\doc\Projetos\Alternativa Marcas e Patentes LTDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="50">
   <si>
     <t>Itens de desenvolvimento do MP</t>
   </si>
@@ -148,6 +148,27 @@
   </si>
   <si>
     <t>não entendi qual seria esta descrição</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retirada do campo obervação no relatório de boletos gerados </t>
+  </si>
+  <si>
+    <t>Correção na quantidade limite de informações carregadas nos relatório de contas a receber e boletos gerados</t>
+  </si>
+  <si>
+    <t>Melhoria no leiaute do boleto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permitir gerar itens financeiros e posteriormente gerar as contas a receber </t>
+  </si>
+  <si>
+    <t>Permitir cadastrar mais de um e-mail para uma pessoa e poder editá-los</t>
+  </si>
+  <si>
+    <t>Criar opção que permite cadastrar um contato para cada telefone da pessoa</t>
+  </si>
+  <si>
+    <t>Permitir editar os endereços das pessoas</t>
   </si>
 </sst>
 </file>
@@ -252,9 +273,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
@@ -263,6 +281,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -350,9 +371,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -390,7 +411,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -462,7 +483,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -612,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -629,13 +650,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -995,33 +1016,33 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="10" t="s">
+      <c r="B28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="10" t="s">
+      <c r="D28" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="9" t="s">
+      <c r="B29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1053,6 +1074,104 @@
         <v>10</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tratamento de um novo formato do número do processo * Correção na filtragem do despacho da patente
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Itens de desenvolvimento.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
   <si>
     <t>Itens de desenvolvimento do MP</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>Permitir editar os endereços das pessoas</t>
+  </si>
+  <si>
+    <t>Filtragem incorreta ao buscar os despachos de patentes no cadastro do processo</t>
+  </si>
+  <si>
+    <t>Filtragem incorreta das pastas cadastradas</t>
+  </si>
+  <si>
+    <t>Implementado novo tratamento do número do processo na leitura da revista</t>
   </si>
 </sst>
 </file>
@@ -633,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1175,6 +1184,48 @@
         <v>8</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>